<commit_message>
update actual positions and safety signals
</commit_message>
<xml_diff>
--- a/setups/vestibular chair/vPrime/lookup/lookup_table_16_16.xlsx
+++ b/setups/vestibular chair/vPrime/lookup/lookup_table_16_16.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjheckman/Documents/Code/Gitlab/pbtoolbox/setups/vestibular chair/vPrime/lookup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2693C9-1254-2142-A08A-D8204E1636D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFA880D-0894-744D-A19C-4A04B6DED90B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25280" yWindow="460" windowWidth="25280" windowHeight="28340" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1960" windowWidth="16800" windowHeight="20540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagram" sheetId="2" r:id="rId1"/>
@@ -1373,7 +1373,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="95" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1913,7 +1913,7 @@
         <v>90</v>
       </c>
       <c r="C18" s="4">
-        <v>-14</v>
+        <v>-17</v>
       </c>
       <c r="D18" s="1">
         <v>90</v>
@@ -1945,7 +1945,7 @@
         <v>90</v>
       </c>
       <c r="C19" s="4">
-        <v>-12</v>
+        <v>-15</v>
       </c>
       <c r="D19" s="1">
         <v>90</v>
@@ -1977,7 +1977,7 @@
         <v>90</v>
       </c>
       <c r="C20" s="4">
-        <v>-10</v>
+        <v>-13</v>
       </c>
       <c r="D20" s="1">
         <v>90</v>
@@ -2009,7 +2009,7 @@
         <v>90</v>
       </c>
       <c r="C21" s="4">
-        <v>-8</v>
+        <v>-10</v>
       </c>
       <c r="D21" s="1">
         <v>90</v>
@@ -2041,7 +2041,7 @@
         <v>90</v>
       </c>
       <c r="C22" s="4">
-        <v>-6</v>
+        <v>-8</v>
       </c>
       <c r="D22" s="1">
         <v>90</v>
@@ -2073,7 +2073,7 @@
         <v>90</v>
       </c>
       <c r="C23" s="4">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="D23" s="1">
         <v>90</v>
@@ -2105,7 +2105,7 @@
         <v>90</v>
       </c>
       <c r="C24" s="4">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="D24" s="1">
         <v>90</v>
@@ -2201,7 +2201,7 @@
         <v>90</v>
       </c>
       <c r="C27" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D27" s="1">
         <v>90</v>
@@ -2233,7 +2233,7 @@
         <v>90</v>
       </c>
       <c r="C28" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D28" s="1">
         <v>90</v>
@@ -2265,7 +2265,7 @@
         <v>90</v>
       </c>
       <c r="C29" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D29" s="1">
         <v>90</v>
@@ -2297,7 +2297,7 @@
         <v>90</v>
       </c>
       <c r="C30" s="4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D30" s="1">
         <v>90</v>
@@ -2329,7 +2329,7 @@
         <v>90</v>
       </c>
       <c r="C31" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D31" s="1">
         <v>90</v>

</xml_diff>

<commit_message>
update actual positions leds
</commit_message>
<xml_diff>
--- a/setups/vestibular chair/vPrime/lookup/lookup_table_16_16.xlsx
+++ b/setups/vestibular chair/vPrime/lookup/lookup_table_16_16.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjheckman/Documents/Code/Gitlab/pbtoolbox/setups/vestibular chair/vPrime/lookup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFA880D-0894-744D-A19C-4A04B6DED90B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6864EC80-849C-A541-86DC-D685726754A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1960" windowWidth="16800" windowHeight="20540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1373,7 +1373,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="95" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1419,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>-40</v>
+        <v>-42</v>
       </c>
       <c r="C2" s="4">
         <v>0</v>
@@ -1483,7 +1483,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C4" s="4">
         <v>0</v>

</xml_diff>